<commit_message>
Move feature eng to page1 and add list
</commit_message>
<xml_diff>
--- a/Document/Function List & Reference.xlsx
+++ b/Document/Function List & Reference.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MENG-Project\bearings-project-meng\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684A2A65-FD1B-48EC-8385-E64C81EA8AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB0A6BE-5F72-437D-B655-D61584AAB1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Check" sheetId="1" r:id="rId1"/>
+    <sheet name="Feature Engineering" sheetId="2" r:id="rId2"/>
+    <sheet name="Data-Clean" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Function</t>
   </si>
@@ -33,9 +35,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Missing value imputation</t>
-  </si>
-  <si>
     <t>Data type validation</t>
   </si>
   <si>
@@ -52,6 +51,132 @@
   </si>
   <si>
     <t>Missing column validation</t>
+  </si>
+  <si>
+    <t>Missing value validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean </t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>standard deviation</t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>skewness</t>
+  </si>
+  <si>
+    <t>kurtosis</t>
+  </si>
+  <si>
+    <t>square root</t>
+  </si>
+  <si>
+    <t>peak-to-peak range</t>
+  </si>
+  <si>
+    <t>root mean square</t>
+  </si>
+  <si>
+    <t>sum of squares</t>
+  </si>
+  <si>
+    <t>Frequency Domain Feature</t>
+  </si>
+  <si>
+    <t>Time Domain Feature</t>
+  </si>
+  <si>
+    <t>FFT (Fast Fourier Transform)</t>
+  </si>
+  <si>
+    <t>FFT magnitude</t>
+  </si>
+  <si>
+    <t>FFT frequency</t>
+  </si>
+  <si>
+    <t>Power spectrum</t>
+  </si>
+  <si>
+    <t>FFT mean</t>
+  </si>
+  <si>
+    <t>FFT standard deviation</t>
+  </si>
+  <si>
+    <t>FFT maximum</t>
+  </si>
+  <si>
+    <t>FFT frequency of maximum amplitude</t>
+  </si>
+  <si>
+    <t>Spectral centroid</t>
+  </si>
+  <si>
+    <t>Spectral bandwidth</t>
+  </si>
+  <si>
+    <t>Amplitude envelope</t>
+  </si>
+  <si>
+    <t>Phase envelope</t>
+  </si>
+  <si>
+    <t>Log power spectrum</t>
+  </si>
+  <si>
+    <t>Cepstrum</t>
+  </si>
+  <si>
+    <t>Cepstrum mean</t>
+  </si>
+  <si>
+    <t>Cepstrum standard deviation</t>
+  </si>
+  <si>
+    <t>Cepstrum maximum</t>
+  </si>
+  <si>
+    <t>Time Frequency Feature</t>
+  </si>
+  <si>
+    <t>STFT mean</t>
+  </si>
+  <si>
+    <t>STFT standard deviation</t>
+  </si>
+  <si>
+    <t>STFT maximum</t>
+  </si>
+  <si>
+    <t>Wavelet mean</t>
+  </si>
+  <si>
+    <t>Wavelet standard deviation</t>
+  </si>
+  <si>
+    <t>Wavelet maximum</t>
+  </si>
+  <si>
+    <t>Missing Value Imputation</t>
+  </si>
+  <si>
+    <t>Normalization</t>
+  </si>
+  <si>
+    <t>Label Encoding</t>
+  </si>
+  <si>
+    <t>Column Type Regulation</t>
+  </si>
+  <si>
+    <t>Outlier Removal</t>
   </si>
 </sst>
 </file>
@@ -371,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,37 +515,269 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8173648E-2E53-4563-84AB-CFEC73580A9A}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{163BB3F7-1C0E-4652-83E7-85EEF3BAC4E7}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Function List & Reference.xlsx
</commit_message>
<xml_diff>
--- a/Document/Function List & Reference.xlsx
+++ b/Document/Function List & Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MENG-Project\bearings-project-meng\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB0A6BE-5F72-437D-B655-D61584AAB1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97CBB93-1D5D-47CD-907A-73749E7579F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="690" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Check" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>